<commit_message>
updating actuator board order sheet
</commit_message>
<xml_diff>
--- a/Titan Boards/Actuator/Actuator_SP21_electrical_order.xlsx
+++ b/Titan Boards/Actuator/Actuator_SP21_electrical_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\OSU\UWRT\Previous Orders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lappt\Documents\Underwater Robotics\uwrt_electronics\Titan Boards\Actuator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A229DEB-1F41-46DD-B3DA-962F52623299}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE79C78D-9A05-416B-8695-DF7ED343D343}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="93">
   <si>
     <t>Item #</t>
   </si>
@@ -246,6 +246,69 @@
   </si>
   <si>
     <t>ABM3B-16.000MHZ-B2-T</t>
+  </si>
+  <si>
+    <t>Varistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERZ-VF2M270/672899</t>
+  </si>
+  <si>
+    <t>ERZ-VF2M270</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10A225KP8NNNC/3889171</t>
+  </si>
+  <si>
+    <t>CL10A225KP8NNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RMCF0603JT22R0/RMCF0603JT22R0CT-ND/1943150</t>
+  </si>
+  <si>
+    <t>RMCF0603JT22R0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10A105KQ8NNNC/3889122</t>
+  </si>
+  <si>
+    <t>CL10A105KQ8NNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603JT560R/7789982</t>
+  </si>
+  <si>
+    <t>RMCF0603JT560R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10C180JB8NNNC/1276-1089-1-ND/3889175</t>
+  </si>
+  <si>
+    <t>CL10C180JB8NNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL10B104KB8NNNC/1276-1000-1-ND/3889086</t>
+  </si>
+  <si>
+    <t>CL10B104KB8NNNC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/bourns-inc/CR0603-JW-104ELF/CR0603-JW-104ELFCT-ND/3767631</t>
+  </si>
+  <si>
+    <t>CR0603-JW-104ELF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603JT10K0/1943191</t>
+  </si>
+  <si>
+    <t>RMCF0603JT10K0</t>
+  </si>
+  <si>
+    <t>GRT32EC81C476ME13L</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/schurter-inc/1301.9302/486-3458-ND/7602712</t>
   </si>
 </sst>
 </file>
@@ -269,16 +332,19 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -298,6 +364,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -331,7 +398,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +415,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
         <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -389,7 +462,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -451,6 +524,20 @@
     <xf numFmtId="8" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency 2" xfId="4" xr:uid="{3D9B0C57-85EF-4F96-B301-B768AB75FC08}"/>
@@ -460,18 +547,6 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{BB65AEA1-BC94-49FD-992B-0DDB11A7F21F}"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -568,6 +643,18 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -842,7 +929,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:O34" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:O35" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item #" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Item Description" dataDxfId="13"/>
@@ -852,15 +939,15 @@
       <calculatedColumnFormula>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Order From" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="URL to Part Page" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Manufacturer Part #" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Notes" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ordered?" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Purchaser" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Date Ordered" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Purchase Method" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Order #" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Actual Cost" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="URL to Part Page" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Manufacturer Part #" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ordered?" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Purchaser" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Date Ordered" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Purchase Method" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Order #" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Actual Cost" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Form-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1064,33 +1151,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O1000"/>
+  <dimension ref="A1:O1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="126.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
-    <col min="13" max="13" width="16.21875" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" customWidth="1"/>
-    <col min="15" max="15" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="26" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="46.6328125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="126.54296875" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.36328125" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="26" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +1224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1147,18 +1234,22 @@
       <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="7" t="e">
+      <c r="D2" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.2</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="18"/>
+      <c r="G2" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>86</v>
+      </c>
       <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1169,7 +1260,7 @@
       <c r="N2" s="10"/>
       <c r="O2" s="12"/>
     </row>
-    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1179,18 +1270,22 @@
       <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="7" t="e">
+      <c r="D3" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.2</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="18"/>
+      <c r="G3" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>84</v>
+      </c>
       <c r="I3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1201,7 +1296,7 @@
       <c r="N3" s="10"/>
       <c r="O3" s="12"/>
     </row>
-    <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1233,7 +1328,7 @@
       <c r="N4" s="10"/>
       <c r="O4" s="12"/>
     </row>
-    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1254,7 +1349,9 @@
         <v>15</v>
       </c>
       <c r="G5" s="28"/>
-      <c r="H5" s="18"/>
+      <c r="H5" s="38" t="s">
+        <v>91</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1265,7 +1362,7 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1297,7 +1394,7 @@
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
     </row>
-    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1307,18 +1404,22 @@
       <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="D7" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="7" t="e">
+      <c r="D7" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.2</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="18"/>
+      <c r="G7" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>76</v>
+      </c>
       <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1329,7 +1430,7 @@
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
     </row>
-    <row r="8" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1361,7 +1462,7 @@
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
     </row>
-    <row r="9" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1371,18 +1472,22 @@
       <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="7" t="e">
+      <c r="D9" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.1</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="18"/>
+      <c r="G9" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>80</v>
+      </c>
       <c r="I9" s="4" t="s">
         <v>20</v>
       </c>
@@ -1393,7 +1498,7 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
     </row>
-    <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -1425,7 +1530,7 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
     </row>
-    <row r="11" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1457,7 +1562,7 @@
       <c r="N11" s="10"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1489,7 +1594,7 @@
       <c r="N12" s="10"/>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1521,7 +1626,7 @@
       <c r="N13" s="10"/>
       <c r="O13" s="12"/>
     </row>
-    <row r="14" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1544,7 +1649,7 @@
       <c r="G14" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="29" t="s">
         <v>54</v>
       </c>
       <c r="I14" s="4" t="s">
@@ -1557,7 +1662,7 @@
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
     </row>
-    <row r="15" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1593,7 +1698,7 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
     </row>
-    <row r="16" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -1603,18 +1708,22 @@
       <c r="C16" s="4">
         <v>2</v>
       </c>
-      <c r="D16" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="7" t="e">
+      <c r="D16" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.2</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="18"/>
+      <c r="G16" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>78</v>
+      </c>
       <c r="I16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1625,7 +1734,7 @@
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
     </row>
-    <row r="17" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1657,7 +1766,7 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
     </row>
-    <row r="18" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1689,7 +1798,7 @@
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
     </row>
-    <row r="19" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13">
         <v>18</v>
       </c>
@@ -1699,18 +1808,22 @@
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="7" t="e">
+      <c r="D19" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.1</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="18"/>
+      <c r="G19" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>82</v>
+      </c>
       <c r="I19" s="4" t="s">
         <v>20</v>
       </c>
@@ -1721,7 +1834,7 @@
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -1753,7 +1866,7 @@
       <c r="N20" s="10"/>
       <c r="O20" s="12"/>
     </row>
-    <row r="21" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1785,7 +1898,7 @@
       <c r="N21" s="10"/>
       <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -1817,7 +1930,7 @@
       <c r="N22" s="10"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1827,18 +1940,22 @@
       <c r="C23" s="4">
         <v>4</v>
       </c>
-      <c r="D23" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="7" t="e">
+      <c r="D23" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.4</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="18"/>
+      <c r="G23" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>90</v>
+      </c>
       <c r="I23" s="4" t="s">
         <v>20</v>
       </c>
@@ -1849,7 +1966,7 @@
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
     </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1859,18 +1976,22 @@
       <c r="C24" s="4">
         <v>2</v>
       </c>
-      <c r="D24" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="7" t="e">
+      <c r="D24" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="E24" s="7">
         <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>0.2</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="18"/>
+      <c r="G24" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>88</v>
+      </c>
       <c r="I24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1881,7 +2002,7 @@
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
     </row>
-    <row r="25" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1901,7 +2022,9 @@
       <c r="F25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="28"/>
+      <c r="G25" s="37" t="s">
+        <v>92</v>
+      </c>
       <c r="H25" s="18"/>
       <c r="I25" s="4" t="s">
         <v>20</v>
@@ -1913,7 +2036,7 @@
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
     </row>
-    <row r="26" spans="1:15" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -1949,7 +2072,7 @@
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
     </row>
-    <row r="27" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1985,7 +2108,7 @@
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
     </row>
-    <row r="28" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13">
         <v>27</v>
       </c>
@@ -2021,7 +2144,7 @@
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
     </row>
-    <row r="29" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2057,7 +2180,7 @@
       <c r="N29" s="10"/>
       <c r="O29" s="12"/>
     </row>
-    <row r="30" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2093,7 +2216,7 @@
       <c r="N30" s="10"/>
       <c r="O30" s="12"/>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2129,7 +2252,7 @@
       <c r="N31" s="10"/>
       <c r="O31" s="12"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2165,7 +2288,7 @@
       <c r="N32" s="10"/>
       <c r="O32" s="12"/>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2201,7 +2324,7 @@
       <c r="N33" s="10"/>
       <c r="O33" s="12"/>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2237,998 +2360,1034 @@
       <c r="N34" s="10"/>
       <c r="O34" s="12"/>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="6">
+        <v>6</v>
+      </c>
+      <c r="D35" s="14">
+        <v>1.55</v>
+      </c>
+      <c r="E35" s="7">
+        <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="9"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="12"/>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="25" t="e">
-        <f>SUBTOTAL(109,Form!$E$2:$E$34)</f>
+      <c r="B36" s="19"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="25" t="e">
+        <f>SUBTOTAL(109,Form!$E$2:$E$35)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2" t="s">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O35" s="3">
+      <c r="O36" s="3">
         <f>SUBTOTAL(109,Form!$O$2:$O$10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Titan actuator, added 22mF caps
</commit_message>
<xml_diff>
--- a/Titan Boards/Actuator/Actuator_SP21_electrical_order.xlsx
+++ b/Titan Boards/Actuator/Actuator_SP21_electrical_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\OSU\UWRT\uwrt_electronics\Titan Boards\Actuator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA25E3-57B8-4415-BEDB-5B018B8C9907}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA4E8F-D799-4DB4-8909-AB8C63C61133}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="120">
   <si>
     <t>Item #</t>
   </si>
@@ -381,6 +381,15 @@
   </si>
   <si>
     <t>RNCP1206FTD1R00</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/UVK1E223MRD/2539394</t>
+  </si>
+  <si>
+    <t>UVK1E223MRD</t>
+  </si>
+  <si>
+    <t>Repeat part from total order</t>
   </si>
 </sst>
 </file>
@@ -528,7 +537,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -601,6 +610,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1219,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1370,20 +1382,24 @@
         <v>22</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="6" t="e">
-        <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
-        <v>#VALUE!</v>
+        <v>2</v>
+      </c>
+      <c r="D4" s="29">
+        <v>5.85</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Table_1[[#This Row],[Cost per Item]]*Table_1[[#This Row],[Quantity]]</f>
+        <v>11.7</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="16"/>
+      <c r="G4" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
       <c r="I4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1450,7 +1466,9 @@
       <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H6" s="16"/>
       <c r="I6" s="4" t="s">
         <v>20</v>
@@ -1518,7 +1536,9 @@
       <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H8" s="16"/>
       <c r="I8" s="4" t="s">
         <v>20</v>
@@ -1586,7 +1606,9 @@
       <c r="F10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="26"/>
+      <c r="G10" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H10" s="16"/>
       <c r="I10" s="4" t="s">
         <v>20</v>
@@ -1618,7 +1640,9 @@
       <c r="F11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H11" s="16"/>
       <c r="I11" s="4" t="s">
         <v>20</v>
@@ -1650,7 +1674,9 @@
       <c r="F12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H12" s="16"/>
       <c r="I12" s="4" t="s">
         <v>20</v>

</xml_diff>